<commit_message>
Changed: names of Chert_type in STA dataset
</commit_message>
<xml_diff>
--- a/analysis/derived_data/ISEA_use-wear_STA.xlsx
+++ b/analysis/derived_data/ISEA_use-wear_STA.xlsx
@@ -588,7 +588,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C2">
@@ -734,7 +734,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C3">
@@ -880,7 +880,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C4">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C5">
@@ -1172,7 +1172,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C6">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C7">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C8">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C9">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C10">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C11">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C12">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C13">
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C14">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C15">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C16">
@@ -2775,7 +2775,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C17">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C18">
@@ -3067,7 +3067,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C19">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C20">
@@ -3359,7 +3359,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C21">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C22">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C23">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C24">
@@ -3943,7 +3943,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C25">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C26">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C27">
@@ -4381,7 +4381,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C28">
@@ -4527,7 +4527,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C29">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C30">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C31">
@@ -4965,7 +4965,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C32">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C33">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C34">
@@ -5403,7 +5403,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C35">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C36">
@@ -5695,7 +5695,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C37">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C38">
@@ -5987,7 +5987,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C39">
@@ -6133,7 +6133,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C40">
@@ -6279,7 +6279,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C41">
@@ -6425,7 +6425,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C42">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C43">
@@ -6717,7 +6717,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C44">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C45">
@@ -7009,7 +7009,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C46">
@@ -7155,7 +7155,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C47">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C48">
@@ -7447,7 +7447,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Coarser</t>
         </is>
       </c>
       <c r="C49">
@@ -7593,7 +7593,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C50">
@@ -7739,7 +7739,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C51">
@@ -7885,7 +7885,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C52">
@@ -8031,7 +8031,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C53">
@@ -8177,7 +8177,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C54">
@@ -8323,7 +8323,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C55">
@@ -8469,7 +8469,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C56">
@@ -8615,7 +8615,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C57">
@@ -8761,7 +8761,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C58">
@@ -8907,7 +8907,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C59">
@@ -9053,7 +9053,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C60">
@@ -9199,7 +9199,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C61">
@@ -9342,7 +9342,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C62">
@@ -9488,7 +9488,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C63">
@@ -9634,7 +9634,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C64">
@@ -9780,7 +9780,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C65">
@@ -9926,7 +9926,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C66">
@@ -10072,7 +10072,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C67">
@@ -10218,7 +10218,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C68">
@@ -10364,7 +10364,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C69">
@@ -10510,7 +10510,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C70">
@@ -10656,7 +10656,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C71">
@@ -10802,7 +10802,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C72">
@@ -10948,7 +10948,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C73">
@@ -11094,7 +11094,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C74">
@@ -11240,7 +11240,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C75">
@@ -11386,7 +11386,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C76">
@@ -11532,7 +11532,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C77">
@@ -11678,7 +11678,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C78">
@@ -11824,7 +11824,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C79">
@@ -11970,7 +11970,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C80">
@@ -12116,7 +12116,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C81">
@@ -12262,7 +12262,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C82">
@@ -12408,7 +12408,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C83">
@@ -12554,7 +12554,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C84">
@@ -12700,7 +12700,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C85">
@@ -12846,7 +12846,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C86">
@@ -12992,7 +12992,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C87">
@@ -13138,7 +13138,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C88">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C89">
@@ -13430,7 +13430,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C90">
@@ -13576,7 +13576,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C91">
@@ -13722,7 +13722,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C92">
@@ -13868,7 +13868,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C93">
@@ -14014,7 +14014,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C94">
@@ -14160,7 +14160,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C95">
@@ -14306,7 +14306,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C96">
@@ -14452,7 +14452,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Finer</t>
         </is>
       </c>
       <c r="C97">

</xml_diff>